<commit_message>
Added cause of death: Collision or Ground
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/AdamsLawIteration.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/AdamsLawIteration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8703BA-85B7-42EE-81AF-8446BACA3985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6933EF7A-6AB5-4AC1-A912-FAAC2EFCFA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
   <si>
     <t>dt</t>
   </si>
@@ -415,6 +415,27 @@
   </si>
   <si>
     <t>[75;75]</t>
+  </si>
+  <si>
+    <t>Scores</t>
+  </si>
+  <si>
+    <t>mapDivResolution</t>
+  </si>
+  <si>
+    <t>mapDivFrameSkip</t>
+  </si>
+  <si>
+    <t>How many boxes the map should be divided into</t>
+  </si>
+  <si>
+    <t>How often to check which divisions have been explored</t>
+  </si>
+  <si>
+    <t>verboseOutput</t>
+  </si>
+  <si>
+    <t>thermalSpawnRange</t>
   </si>
 </sst>
 </file>
@@ -744,10 +765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K94"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -897,12 +918,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -913,7 +934,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -924,7 +945,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -935,7 +956,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -946,28 +967,25 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="2">
-        <v>1000</v>
-      </c>
-      <c r="D26">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>104</v>
       </c>
@@ -975,7 +993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -983,10 +1001,10 @@
         <v>109</v>
       </c>
       <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -994,10 +1012,10 @@
         <v>111</v>
       </c>
       <c r="C29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>112</v>
       </c>
@@ -1005,7 +1023,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>113</v>
       </c>
@@ -1013,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>29</v>
       </c>
@@ -1023,11 +1041,9 @@
         <v>30</v>
       </c>
       <c r="C33" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="D33" s="2">
         <v>0.1</v>
       </c>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
@@ -1061,10 +1077,10 @@
         <v>32</v>
       </c>
       <c r="C37" s="2">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D37">
-        <v>0.05</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
@@ -1290,8 +1306,12 @@
       <c r="C61">
         <v>4</v>
       </c>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="D61" s="4">
+        <v>7</v>
+      </c>
+      <c r="E61" s="4">
+        <v>10</v>
+      </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -1438,166 +1458,212 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A78" s="1" t="s">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B77" t="s">
+        <v>132</v>
+      </c>
+      <c r="C77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B79" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B80" t="s">
+        <v>72</v>
+      </c>
+      <c r="C80" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B81" t="s">
+        <v>133</v>
+      </c>
+      <c r="C81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B82" t="s">
         <v>74</v>
       </c>
-      <c r="C80">
+      <c r="C82">
         <v>50</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>85</v>
-      </c>
-      <c r="B81" t="s">
-        <v>75</v>
-      </c>
-      <c r="C81">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A82" t="s">
-        <v>20</v>
-      </c>
-      <c r="B82" t="s">
-        <v>76</v>
-      </c>
-      <c r="C82">
-        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C84">
-        <v>300</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C85">
-        <v>550</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="B86" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>300</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="B87" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C87">
-        <v>10</v>
+        <v>550</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B88" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C88">
-        <v>0.01</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C89">
-        <v>600</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>82</v>
+      </c>
+      <c r="C90">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91" t="s">
+        <v>83</v>
+      </c>
+      <c r="C91">
+        <v>800</v>
+      </c>
+      <c r="D91">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A92" t="s">
         <v>87</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B92" t="s">
         <v>84</v>
       </c>
-      <c r="C90">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="3"/>
-      <c r="I91" s="3"/>
-      <c r="J91" s="3"/>
-      <c r="K91" s="3"/>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A92" s="1" t="s">
+      <c r="C92">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
+      <c r="J93" s="3"/>
+      <c r="K93" s="3"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A94" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B93" t="s">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B95" t="s">
         <v>91</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C95" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B94" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B96" t="s">
         <v>92</v>
       </c>
-      <c r="C94" t="s">
+      <c r="C96" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A98" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>130</v>
+      </c>
+      <c r="B99" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A100" t="s">
+        <v>131</v>
+      </c>
+      <c r="B100" t="s">
+        <v>129</v>
+      </c>
+      <c r="C100">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set up megarun for baseline
</commit_message>
<xml_diff>
--- a/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/AdamsLawIteration.xlsx
+++ b/matlab/REU_2022/Topic_3_Soaring/Sim_Draft_1/Code_of_Laws/AdamsLawIteration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hombo\Documents\Github Repositories\REU_MatlabSim\matlab\REU_2022\Topic_3_Soaring\Sim_Draft_1\Code_of_Laws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6933EF7A-6AB5-4AC1-A912-FAAC2EFCFA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B410053-153A-48F2-8D94-E646548D243B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="135">
   <si>
     <t>dt</t>
   </si>
@@ -351,9 +351,6 @@
     <t>heightFactorPower</t>
   </si>
   <si>
-    <t>[1600,1600]</t>
-  </si>
-  <si>
     <t>agentControl_Unified</t>
   </si>
   <si>
@@ -408,15 +405,6 @@
     <t>followRadius</t>
   </si>
   <si>
-    <t>[-2000,2000]</t>
-  </si>
-  <si>
-    <t>[-1500,-1500;1500,1500]</t>
-  </si>
-  <si>
-    <t>[75;75]</t>
-  </si>
-  <si>
     <t>Scores</t>
   </si>
   <si>
@@ -436,6 +424,21 @@
   </si>
   <si>
     <t>thermalSpawnRange</t>
+  </si>
+  <si>
+    <t>[-4000,4000]</t>
+  </si>
+  <si>
+    <t>[-3000,-3000;3000,3000]</t>
+  </si>
+  <si>
+    <t>[1100,1500]</t>
+  </si>
+  <si>
+    <t>[150;150]</t>
+  </si>
+  <si>
+    <t>[-3000,3000]</t>
   </si>
 </sst>
 </file>
@@ -765,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -777,12 +780,12 @@
     <col min="2" max="2" width="23.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -792,8 +795,11 @@
       <c r="C2">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -801,10 +807,13 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>7200</v>
+      </c>
+      <c r="D3">
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -814,8 +823,11 @@
       <c r="C4">
         <v>120</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D4">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -823,10 +835,13 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -836,8 +851,11 @@
       <c r="C6">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -845,331 +863,422 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
         <v>94</v>
       </c>
-      <c r="C8" t="b">
+      <c r="C9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
         <v>95</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B10" t="s">
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
         <v>100</v>
       </c>
-      <c r="C10" t="b">
+      <c r="C11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B11" t="s">
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
         <v>101</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="1" t="s">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C14" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C15" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>14</v>
       </c>
       <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>2600</v>
+      </c>
+      <c r="D16">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" s="1" t="s">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="C20" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>132</v>
+      </c>
+      <c r="D21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>21</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>27</v>
       </c>
-      <c r="C22">
+      <c r="C23">
         <v>9.81</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A24" s="1" t="s">
+      <c r="D23">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
+      <c r="C27" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
         <v>104</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" t="s">
         <v>108</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>109</v>
       </c>
-      <c r="C28">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="B30" t="s">
         <v>110</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
         <v>111</v>
       </c>
-      <c r="C29">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B30" t="s">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
         <v>112</v>
       </c>
-      <c r="C30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
-        <v>113</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A32" s="1" t="s">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B33" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C34" s="2">
         <v>0.1</v>
       </c>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>114</v>
-      </c>
-      <c r="B34" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34">
-        <v>200</v>
+      <c r="D34" s="2">
+        <v>0.1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35">
+        <v>50</v>
+      </c>
+      <c r="D35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" t="s">
         <v>115</v>
       </c>
-      <c r="B35" t="s">
-        <v>116</v>
-      </c>
-      <c r="C35">
+      <c r="C36">
         <v>-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A36" s="1" t="s">
+      <c r="D36">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="2">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D37">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>117</v>
-      </c>
-      <c r="B38" t="s">
-        <v>118</v>
-      </c>
-      <c r="C38">
-        <v>200</v>
+      <c r="C38" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="D38" s="2">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" t="s">
         <v>119</v>
       </c>
-      <c r="B39" t="s">
-        <v>120</v>
-      </c>
-      <c r="C39">
+      <c r="C40">
         <v>-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" s="1" t="s">
+      <c r="D40">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" s="1" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A41" s="1"/>
-      <c r="B41" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="2">
-        <v>5.9999999999999999E-24</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" s="1"/>
       <c r="B42" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="C42">
-        <v>6</v>
+        <v>9.9999999999999991E-22</v>
+      </c>
+      <c r="D42">
+        <v>9.9999999999999991E-22</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="1"/>
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C43">
+        <v>5</v>
+      </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B44" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
         <v>38</v>
       </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>41</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>39</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
+      <c r="D46" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>98</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>97</v>
       </c>
-      <c r="C48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D49" s="4"/>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
@@ -1178,42 +1287,37 @@
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A50" s="1" t="s">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A51" s="1" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>14</v>
-      </c>
-      <c r="B51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C51">
-        <v>1000</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52">
-        <v>10</v>
+        <v>1000</v>
+      </c>
+      <c r="D52">
+        <v>1000</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
@@ -1221,24 +1325,28 @@
         <v>20</v>
       </c>
       <c r="B54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C54">
-        <v>13</v>
+        <v>8</v>
+      </c>
+      <c r="D54">
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C55">
-        <f>-1/12*PI()</f>
-        <v>-0.26179938779914941</v>
-      </c>
-      <c r="D55" s="4"/>
+        <v>13</v>
+      </c>
+      <c r="D55">
+        <v>13</v>
+      </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -1252,66 +1360,76 @@
         <v>49</v>
       </c>
       <c r="B56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C56">
-        <f>1/12*PI()</f>
-        <v>0.26179938779914941</v>
+        <v>-0.26179938779914941</v>
+      </c>
+      <c r="D56">
+        <v>-0.26179938779914941</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
+        <v>49</v>
+      </c>
+      <c r="B57" t="s">
+        <v>50</v>
+      </c>
+      <c r="C57">
+        <v>0.26179938779914941</v>
+      </c>
+      <c r="D57">
+        <v>0.26179938779914941</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>52</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>51</v>
       </c>
-      <c r="C57">
-        <f t="shared" ref="C57" si="0">11/6*PI()</f>
+      <c r="C58">
         <v>5.7595865315812871</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B58" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58">
-        <v>-1.8429999999999998E-2</v>
+      <c r="D58">
+        <v>5.7595865315812871</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C59">
-        <v>0.37819999999999998</v>
+        <v>-1.8429999999999998E-2</v>
+      </c>
+      <c r="D59">
+        <v>-1.8429999999999998E-2</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="C60">
+        <v>0.37819999999999998</v>
+      </c>
+      <c r="D60">
+        <v>0.37819999999999998</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B61" t="s">
         <v>55</v>
       </c>
-      <c r="C60">
-        <f t="shared" ref="C60" si="1">-2.3782</f>
+      <c r="C61">
         <v>-2.3782000000000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B61" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61">
-        <v>4</v>
-      </c>
-      <c r="D61" s="4">
-        <v>7</v>
-      </c>
-      <c r="E61" s="4">
-        <v>10</v>
-      </c>
+      <c r="D61">
+        <v>-2.3782000000000001</v>
+      </c>
+      <c r="E61" s="4"/>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -1319,11 +1437,21 @@
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
     </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>14</v>
+      </c>
+      <c r="B62" t="s">
+        <v>93</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+    </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A63" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D63" s="2"/>
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -1333,13 +1461,9 @@
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B64" t="s">
-        <v>57</v>
-      </c>
-      <c r="C64" t="s">
-        <v>58</v>
-      </c>
-      <c r="D64" s="2"/>
+      <c r="A64" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -1350,12 +1474,14 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
-      </c>
-      <c r="D65" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="D65" t="s">
+        <v>58</v>
+      </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -1366,104 +1492,140 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
+        <v>59</v>
+      </c>
+      <c r="C66" t="s">
+        <v>60</v>
+      </c>
+      <c r="D66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B67" t="s">
         <v>61</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C67" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+      <c r="D67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>64</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>63</v>
       </c>
-      <c r="C67" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B68" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="3" t="b">
-        <v>1</v>
+      <c r="C68" t="s">
+        <v>133</v>
+      </c>
+      <c r="D68" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B69" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="3" t="b">
-        <v>1</v>
+        <v>65</v>
+      </c>
+      <c r="C69" t="b">
+        <v>0</v>
+      </c>
+      <c r="D69" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
-        <v>67</v>
-      </c>
-      <c r="C70" s="3" t="b">
-        <v>1</v>
+        <v>66</v>
+      </c>
+      <c r="C70" t="b">
+        <v>0</v>
+      </c>
+      <c r="D70" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B71" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C71" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D71" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B72" t="s">
-        <v>69</v>
-      </c>
-      <c r="C72" s="3" t="b">
+        <v>68</v>
+      </c>
+      <c r="C72" t="b">
+        <v>1</v>
+      </c>
+      <c r="D72" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B73" t="s">
+        <v>69</v>
+      </c>
+      <c r="C73" t="b">
+        <v>0</v>
+      </c>
+      <c r="D73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="B74" t="s">
         <v>70</v>
       </c>
-      <c r="C73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>122</v>
-      </c>
-      <c r="B74" t="s">
+      <c r="C74" t="b">
+        <v>0</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>121</v>
+      </c>
+      <c r="B75" t="s">
         <v>102</v>
       </c>
-      <c r="C74" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B75" t="s">
-        <v>123</v>
-      </c>
-      <c r="C75">
-        <v>2500</v>
+      <c r="C75" t="b">
+        <v>0</v>
+      </c>
+      <c r="D75" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B76" t="s">
-        <v>103</v>
-      </c>
-      <c r="C76" t="b">
-        <v>1</v>
+        <v>122</v>
+      </c>
+      <c r="C76">
+        <v>2500</v>
+      </c>
+      <c r="D76">
+        <v>2500</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B77" t="s">
-        <v>132</v>
+        <v>103</v>
       </c>
       <c r="C77" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D77" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.45">
@@ -1472,19 +1634,26 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A80" s="1"/>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>129</v>
       </c>
       <c r="C80" t="s">
-        <v>73</v>
+        <v>134</v>
+      </c>
+      <c r="D80" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B81" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
       <c r="C81" t="s">
-        <v>124</v>
+        <v>73</v>
+      </c>
+      <c r="D81" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.45">
@@ -1492,7 +1661,10 @@
         <v>74</v>
       </c>
       <c r="C82">
-        <v>50</v>
+        <v>200</v>
+      </c>
+      <c r="D82">
+        <v>200</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.45">
@@ -1505,6 +1677,9 @@
       <c r="C83">
         <v>50</v>
       </c>
+      <c r="D83">
+        <v>50</v>
+      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
@@ -1516,6 +1691,9 @@
       <c r="C84">
         <v>0</v>
       </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
@@ -1527,6 +1705,9 @@
       <c r="C85">
         <v>0</v>
       </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
@@ -1538,6 +1719,9 @@
       <c r="C86">
         <v>300</v>
       </c>
+      <c r="D86">
+        <v>300</v>
+      </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
@@ -1549,6 +1733,9 @@
       <c r="C87">
         <v>550</v>
       </c>
+      <c r="D87">
+        <v>550</v>
+      </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
@@ -1560,6 +1747,9 @@
       <c r="C88">
         <v>3</v>
       </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
@@ -1571,6 +1761,9 @@
       <c r="C89">
         <v>10</v>
       </c>
+      <c r="D89">
+        <v>10</v>
+      </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
@@ -1580,7 +1773,10 @@
         <v>82</v>
       </c>
       <c r="C90">
-        <v>0.05</v>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D90">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.45">
@@ -1594,7 +1790,7 @@
         <v>800</v>
       </c>
       <c r="D91">
-        <v>1000</v>
+        <v>800</v>
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.45">
@@ -1605,11 +1801,13 @@
         <v>84</v>
       </c>
       <c r="C92">
-        <v>800</v>
+        <v>600</v>
+      </c>
+      <c r="D92">
+        <v>600</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D93" s="3"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -1628,7 +1826,10 @@
         <v>91</v>
       </c>
       <c r="C95" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="D95" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.45">
@@ -1636,35 +1837,68 @@
         <v>92</v>
       </c>
       <c r="C96" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+        <v>106</v>
+      </c>
+      <c r="D96" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A98" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B99" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C99">
         <v>10</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B100" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C100">
         <v>10</v>
       </c>
+      <c r="D100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B121" s="1"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B136" s="1"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B137" s="1"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B151" s="1"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B155" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>